<commit_message>
add 2 field hostname and user change gridview and add one action edit menu add/edit and detail aset adit menu references
</commit_message>
<xml_diff>
--- a/InvSystem/obj/Release/Package/PackageTmp/template/TemplateUpload.xlsx
+++ b/InvSystem/obj/Release/Package/PackageTmp/template/TemplateUpload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dede\WORK\Case\Inventory IT\Sample\Others\Sample\Empty\Final\InvSystem\InvSystem\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dede.antini\Desktop\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD81A62-62A5-4B91-98D3-5F13798C2113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD62C1A2-A709-4827-BF5C-E98AD7DBC337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1D99F045-E079-4AC9-AE53-31F786CA0A7E}"/>
   </bookViews>
@@ -40,15 +40,18 @@
     <author>tc={7F27B1DE-8181-47F6-8708-101C366D70B1}</author>
     <author>tc={34C6C5AE-B4C7-4B85-9E03-A4C316CA836C}</author>
     <author>tc={8EAED8FC-8986-473A-8E7C-760B257FB3B2}</author>
+    <author>tc={7A3E5C77-11E5-43C4-9BB3-57FF362712F0}</author>
     <author>tc={E91A35A8-C527-465D-89F0-F256743211C1}</author>
     <author>tc={597EACD4-7D96-4343-9839-90C49C0D801C}</author>
     <author>tc={EC6CFADB-FDB6-4686-AF71-D9972AD5BB61}</author>
     <author>tc={6E6F1860-48D6-4180-9BFB-66CD56B5D00D}</author>
+    <author>tc={F5D6FFB8-1100-4175-BD9B-B2031848A574}</author>
     <author>tc={F0908237-959A-4F39-92C9-6A75562F1BCE}</author>
     <author>tc={01DD0CBD-7AFB-4A0C-B267-9699F5EA165B}</author>
     <author>tc={74CC5E81-7BB4-4CB2-995E-9C13663A6644}</author>
     <author>tc={C6E515DF-DF5A-4B4B-B861-A5F9089F4CB5}</author>
     <author>tc={AAB51C24-7FFF-4657-8871-6FE7E675B9C6}</author>
+    <author>tc={E0EE542A-2B38-4FD5-BE35-265C6F9707CE}</author>
     <author>tc={B2684FF3-88DA-4455-8EDD-D82B4A8F8C5B}</author>
     <author>tc={45BDAA8A-9287-4EFC-B868-B765A2E24A0D}</author>
     <author>tc={DF51428B-CFC3-4522-8211-C03B9053A0C5}</author>
@@ -74,7 +77,6 @@
     <author>tc={A428C808-FB23-4D94-8784-ABA1CEE99BDD}</author>
     <author>tc={60EF7FD3-3C14-42CD-B72B-D2C5F8E0620D}</author>
     <author>tc={8C293A15-0351-42E6-8CA8-98C96A5A6B59}</author>
-    <author>tc={7A3E5C77-11E5-43C4-9BB3-57FF362712F0}</author>
     <author>tc={A09E11A4-C76F-4A0C-859C-FA187A5EB275}</author>
     <author>tc={FFFADD91-B16E-4BB6-A356-9441A872E4DC}</author>
     <author>tc={43733F07-F0C8-44AA-9B73-7EF3968FCF36}</author>
@@ -115,34 +117,63 @@
     Length: 20 character</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{E91A35A8-C527-465D-89F0-F256743211C1}">
+    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{7A3E5C77-11E5-43C4-9BB3-57FF362712F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Value: Code Reference dengan reference type = Health
+E001=NA
+E002=Green
+E003=Purple
+E004=Yellow
+E005=Red</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{E91A35A8-C527-465D-89F0-F256743211C1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Placement Characteristic
-ex: P001</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{597EACD4-7D96-4343-9839-90C49C0D801C}">
+P001= NA
+P002=Stationary
+P003=Carry By Employee</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{597EACD4-7D96-4343-9839-90C49C0D801C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Location
-ex: L001</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{EC6CFADB-FDB6-4686-AF71-D9972AD5BB61}">
+L001=NA
+L002=Lubuk Naga
+L003=Jakarta
+L004=Ajibata
+L005=Pangambatan
+L006=Lontung
+L007=Sirungkungon
+L008=Silimalombu</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{EC6CFADB-FDB6-4686-AF71-D9972AD5BB61}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Area
-ex: A001</t>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{6E6F1860-48D6-4180-9BFB-66CD56B5D00D}">
+A001=NA
+A002=Processing Plant
+A003=Office	
+A004=Guest House
+A005=Feedmill	
+A006=Hatchery	
+A007=Landing Site 1	
+A008=Landing Site 2</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{6E6F1860-48D6-4180-9BFB-66CD56B5D00D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -150,25 +181,68 @@
     length: 500 character</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{F0908237-959A-4F39-92C9-6A75562F1BCE}">
+    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{F5D6FFB8-1100-4175-BD9B-B2031848A574}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Length: 50 character</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{F0908237-959A-4F39-92C9-6A75562F1BCE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Asset Type
-ex: S001</t>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{01DD0CBD-7AFB-4A0C-B267-9699F5EA165B}">
+S001=NA
+S002=Laptop
+S003=Printer Wirelless
+S004=Projector
+S005=Router
+S006=Access Point
+S007=UPS
+S008=Switch 10/100/1000
+S009=Camera Coaxial
+S010=Camera IP
+S011=DVR
+S012=NVR
+S013=Switch 10/100
+S014=Module SFP
+S015=Module Converter (MC)
+S016=Printer
+S017=Printer Lan
+S018=Stabillizer
+S019=HDD Casing 2.4
+S020=HDD Casing 3.5
+S021=Server</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{01DD0CBD-7AFB-4A0C-B267-9699F5EA165B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Asset Brand
-ex: B001</t>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{74CC5E81-7BB4-4CB2-995E-9C13663A6644}">
+B001=NA
+B002=Lenovo
+B003=Asus
+B004=Acer
+B005=HP
+B006=Samsung
+B007=Orico
+B008=Bardi
+B009=IBM
+B010=Fortinet
+B011=Mikrotik
+B012=Unifi
+B013=TP-Link
+B014=D-Link
+B015=Ruijie
+B016=Huawei</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{74CC5E81-7BB4-4CB2-995E-9C13663A6644}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -176,7 +250,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{C6E515DF-DF5A-4B4B-B861-A5F9089F4CB5}">
+    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{C6E515DF-DF5A-4B4B-B861-A5F9089F4CB5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -184,7 +258,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{AAB51C24-7FFF-4657-8871-6FE7E675B9C6}">
+    <comment ref="O1" authorId="14" shapeId="0" xr:uid="{AAB51C24-7FFF-4657-8871-6FE7E675B9C6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -192,16 +266,34 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{B2684FF3-88DA-4455-8EDD-D82B4A8F8C5B}">
+    <comment ref="P1" authorId="15" shapeId="0" xr:uid="{E0EE542A-2B38-4FD5-BE35-265C6F9707CE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Length: 50 character</t>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="16" shapeId="0" xr:uid="{B2684FF3-88DA-4455-8EDD-D82B4A8F8C5B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Color
-ex: C001</t>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="14" shapeId="0" xr:uid="{45BDAA8A-9287-4EFC-B868-B765A2E24A0D}">
+C001=NA
+C002=Red
+C003=Black
+C004=White
+C005=Yellow
+C006=Green
+C007=Blue
+C008=Transparant
+C009=Silver
+C010=Grey
+C011=Brown</t>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="17" shapeId="0" xr:uid="{45BDAA8A-9287-4EFC-B868-B765A2E24A0D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -209,7 +301,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="P1" authorId="15" shapeId="0" xr:uid="{DF51428B-CFC3-4522-8211-C03B9053A0C5}">
+    <comment ref="S1" authorId="18" shapeId="0" xr:uid="{DF51428B-CFC3-4522-8211-C03B9053A0C5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -217,16 +309,18 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="16" shapeId="0" xr:uid="{7EC55F5A-57D1-4574-BF47-D7C5393AEC8A}">
+    <comment ref="T1" authorId="19" shapeId="0" xr:uid="{7EC55F5A-57D1-4574-BF47-D7C5393AEC8A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Touch Screen
-ex: U001</t>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="17" shapeId="0" xr:uid="{B9A66794-AAE1-42F0-8013-9919087BCA06}">
+U001=NA
+U002=Yes
+U003=No</t>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="20" shapeId="0" xr:uid="{B9A66794-AAE1-42F0-8013-9919087BCA06}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -234,25 +328,32 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="S1" authorId="18" shapeId="0" xr:uid="{DDED7A91-AA30-4D58-AAA0-043D8C86F9FB}">
+    <comment ref="V1" authorId="21" shapeId="0" xr:uid="{DDED7A91-AA30-4D58-AAA0-043D8C86F9FB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = VGA Brand
-ex: V001</t>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="19" shapeId="0" xr:uid="{2095BA9B-35A9-4335-900C-D1B5D9E993DC}">
+V001=NA
+V002=NVidia
+V003=Radeon
+V004=ATI Radeon
+V005=Intel Iris
+V006=Intel</t>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="22" shapeId="0" xr:uid="{2095BA9B-35A9-4335-900C-D1B5D9E993DC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = VGA Type
-ex: G001</t>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="20" shapeId="0" xr:uid="{D517ECB9-A8D2-44AB-8307-4A81DD24DF09}">
+G001=NA
+G002=DDR4
+G003=DDR5</t>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="23" shapeId="0" xr:uid="{D517ECB9-A8D2-44AB-8307-4A81DD24DF09}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -260,16 +361,22 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="V1" authorId="21" shapeId="0" xr:uid="{1725C053-09E3-4137-838D-10A62C6E1FB7}">
+    <comment ref="Y1" authorId="24" shapeId="0" xr:uid="{1725C053-09E3-4137-838D-10A62C6E1FB7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = RAM Type
-ex: R001</t>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="22" shapeId="0" xr:uid="{A4CF5CBF-0D29-4906-9E59-F15A66C189B6}">
+R001=NA
+R002=DDR
+R003=DDR2
+R004=DDR3
+R005=DDR3L
+R006=DDR4
+R007=DDR5</t>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="25" shapeId="0" xr:uid="{A4CF5CBF-0D29-4906-9E59-F15A66C189B6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -277,7 +384,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="23" shapeId="0" xr:uid="{38DDC78F-D356-4C96-A5A5-09E52D4E2997}">
+    <comment ref="AA1" authorId="26" shapeId="0" xr:uid="{38DDC78F-D356-4C96-A5A5-09E52D4E2997}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -285,16 +392,20 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="24" shapeId="0" xr:uid="{075415BC-24F5-4DF0-98AB-7B118D84DD9E}">
+    <comment ref="AB1" authorId="27" shapeId="0" xr:uid="{075415BC-24F5-4DF0-98AB-7B118D84DD9E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Storage Type
-ex: T001</t>
-      </text>
-    </comment>
-    <comment ref="Z1" authorId="25" shapeId="0" xr:uid="{2856AB68-D1EA-4362-B4C4-29E912499609}">
+T001=NA
+T002=HDD
+T003=SSD SATA
+T004=SSD NVME
+T005=SSD M.2</t>
+      </text>
+    </comment>
+    <comment ref="AC1" authorId="28" shapeId="0" xr:uid="{2856AB68-D1EA-4362-B4C4-29E912499609}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -302,16 +413,18 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="AA1" authorId="26" shapeId="0" xr:uid="{F0769AF9-C4CA-4934-AA23-2EAD37E490F5}">
+    <comment ref="AD1" authorId="29" shapeId="0" xr:uid="{F0769AF9-C4CA-4934-AA23-2EAD37E490F5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Charger Type
-ex: H001</t>
-      </text>
-    </comment>
-    <comment ref="AB1" authorId="27" shapeId="0" xr:uid="{AF93CD7A-3953-4AA0-B8DE-11E97FF8EB47}">
+H001=NA
+H002=KW
+H003=ORIGINAL</t>
+      </text>
+    </comment>
+    <comment ref="AE1" authorId="30" shapeId="0" xr:uid="{AF93CD7A-3953-4AA0-B8DE-11E97FF8EB47}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -319,7 +432,7 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="AC1" authorId="28" shapeId="0" xr:uid="{7F72F8FD-20FF-47DF-8A5A-95CE7058FC86}">
+    <comment ref="AF1" authorId="31" shapeId="0" xr:uid="{7F72F8FD-20FF-47DF-8A5A-95CE7058FC86}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -327,7 +440,7 @@
     Type Numeric(10,4) (Ex: 10.45)</t>
       </text>
     </comment>
-    <comment ref="AD1" authorId="29" shapeId="0" xr:uid="{9FB7C414-E930-42FA-BF5F-1858645CA7FE}">
+    <comment ref="AG1" authorId="32" shapeId="0" xr:uid="{9FB7C414-E930-42FA-BF5F-1858645CA7FE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -335,7 +448,7 @@
     Type Numeric(10,4) (Ex: 10.45)</t>
       </text>
     </comment>
-    <comment ref="AE1" authorId="30" shapeId="0" xr:uid="{FF0B3A1E-E657-4B84-8260-6CAE71429588}">
+    <comment ref="AH1" authorId="33" shapeId="0" xr:uid="{FF0B3A1E-E657-4B84-8260-6CAE71429588}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -343,7 +456,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="AF1" authorId="31" shapeId="0" xr:uid="{7ADE5977-2A89-45C2-8D2A-2A2B9E8BF5FB}">
+    <comment ref="AI1" authorId="34" shapeId="0" xr:uid="{7ADE5977-2A89-45C2-8D2A-2A2B9E8BF5FB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -351,7 +464,7 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="AG1" authorId="32" shapeId="0" xr:uid="{D2759B04-5250-467C-B703-A7DEB69F88A6}">
+    <comment ref="AJ1" authorId="35" shapeId="0" xr:uid="{D2759B04-5250-467C-B703-A7DEB69F88A6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -359,7 +472,7 @@
     Type Numeric(10,4) (Ex: 10.45)</t>
       </text>
     </comment>
-    <comment ref="AH1" authorId="33" shapeId="0" xr:uid="{C94C18E7-FE0D-4823-BD39-A2770272C0AF}">
+    <comment ref="AK1" authorId="36" shapeId="0" xr:uid="{C94C18E7-FE0D-4823-BD39-A2770272C0AF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -367,7 +480,7 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="AI1" authorId="34" shapeId="0" xr:uid="{348202B7-A2B1-418B-868E-8D959F449C25}">
+    <comment ref="AL1" authorId="37" shapeId="0" xr:uid="{348202B7-A2B1-418B-868E-8D959F449C25}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -375,16 +488,20 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="35" shapeId="0" xr:uid="{A428C808-FB23-4D94-8784-ABA1CEE99BDD}">
+    <comment ref="AM1" authorId="38" shapeId="0" xr:uid="{A428C808-FB23-4D94-8784-ABA1CEE99BDD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Chasing Type
-ex: N001</t>
-      </text>
-    </comment>
-    <comment ref="AK1" authorId="36" shapeId="0" xr:uid="{60EF7FD3-3C14-42CD-B72B-D2C5F8E0620D}">
+N001=NA
+N002=Micro
+N003=Mini
+N004=Medium
+N005=Full</t>
+      </text>
+    </comment>
+    <comment ref="AN1" authorId="39" shapeId="0" xr:uid="{60EF7FD3-3C14-42CD-B72B-D2C5F8E0620D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -392,7 +509,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="AL1" authorId="37" shapeId="0" xr:uid="{8C293A15-0351-42E6-8CA8-98C96A5A6B59}">
+    <comment ref="AO1" authorId="40" shapeId="0" xr:uid="{8C293A15-0351-42E6-8CA8-98C96A5A6B59}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -400,25 +517,31 @@
     Type Integer (Ex: 10)</t>
       </text>
     </comment>
-    <comment ref="AM1" authorId="38" shapeId="0" xr:uid="{7A3E5C77-11E5-43C4-9BB3-57FF362712F0}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Value: Code Reference dengan reference type = Health
-ex: E001</t>
-      </text>
-    </comment>
-    <comment ref="AN1" authorId="39" shapeId="0" xr:uid="{A09E11A4-C76F-4A0C-859C-FA187A5EB275}">
+    <comment ref="AP1" authorId="41" shapeId="0" xr:uid="{A09E11A4-C76F-4A0C-859C-FA187A5EB275}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Value: Code Reference dengan reference type = Operating System
-ex: O001</t>
-      </text>
-    </comment>
-    <comment ref="AO1" authorId="40" shapeId="0" xr:uid="{FFFADD91-B16E-4BB6-A356-9441A872E4DC}">
+O001=NA
+O002=Windows 7
+O003=Windows 8
+O004=Windows 8.1
+O005=Windows 10
+O006=Windows 11
+O007=Windows Ce
+O008=Windows Server 2008
+O009=Windows Server 2008 R2
+O010=Windows Server 2012
+O011=Windows Server 2012 R2
+O012=Windows Server 2016
+O013=Windows Server 2016 R2
+O014=Linux Centos
+O015=VMware Esxi 6.7.0
+O016=VMware Esxi 6.5.0</t>
+      </text>
+    </comment>
+    <comment ref="AQ1" authorId="42" shapeId="0" xr:uid="{FFFADD91-B16E-4BB6-A356-9441A872E4DC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -426,7 +549,7 @@
     Length: 300 character</t>
       </text>
     </comment>
-    <comment ref="AP1" authorId="41" shapeId="0" xr:uid="{43733F07-F0C8-44AA-9B73-7EF3968FCF36}">
+    <comment ref="AR1" authorId="43" shapeId="0" xr:uid="{43733F07-F0C8-44AA-9B73-7EF3968FCF36}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -434,7 +557,7 @@
     Length: 30 character</t>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="42" shapeId="0" xr:uid="{17AC62A8-155A-4950-9CF9-9B05E6C208B0}">
+    <comment ref="AS1" authorId="44" shapeId="0" xr:uid="{17AC62A8-155A-4950-9CF9-9B05E6C208B0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -442,7 +565,7 @@
     Length: 30 character</t>
       </text>
     </comment>
-    <comment ref="AR1" authorId="43" shapeId="0" xr:uid="{00B93DB6-64C2-4327-ABF2-D95ED41C5701}">
+    <comment ref="AT1" authorId="45" shapeId="0" xr:uid="{00B93DB6-64C2-4327-ABF2-D95ED41C5701}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -450,7 +573,7 @@
     Length: 30 character</t>
       </text>
     </comment>
-    <comment ref="AS1" authorId="44" shapeId="0" xr:uid="{95761249-7F6D-48C5-A51E-6F025B5E6978}">
+    <comment ref="AU1" authorId="46" shapeId="0" xr:uid="{95761249-7F6D-48C5-A51E-6F025B5E6978}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -463,7 +586,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>AssetDesc</t>
   </si>
@@ -598,6 +721,12 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>HostName</t>
   </si>
 </sst>
 </file>
@@ -605,7 +734,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -619,7 +748,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -644,7 +773,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,142 +1106,253 @@
   <threadedComment ref="D1" dT="2022-11-25T02:07:16.93" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{8EAED8FC-8986-473A-8E7C-760B257FB3B2}">
     <text>Length: 20 character</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2022-11-25T02:09:58.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{E91A35A8-C527-465D-89F0-F256743211C1}">
+  <threadedComment ref="E1" dT="2022-11-25T02:30:49.89" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7A3E5C77-11E5-43C4-9BB3-57FF362712F0}">
+    <text>Value: Code Reference dengan reference type = Health
+E001=NA
+E002=Green
+E003=Purple
+E004=Yellow
+E005=Red</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2022-11-25T02:09:58.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{E91A35A8-C527-465D-89F0-F256743211C1}">
     <text>Value: Code Reference dengan reference type = Placement Characteristic
-ex: P001</text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2022-11-25T02:10:27.71" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{597EACD4-7D96-4343-9839-90C49C0D801C}">
+P001= NA
+P002=Stationary
+P003=Carry By Employee</text>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2022-11-25T02:10:27.71" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{597EACD4-7D96-4343-9839-90C49C0D801C}">
     <text>Value: Code Reference dengan reference type = Location
-ex: L001</text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2022-11-25T02:10:51.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{EC6CFADB-FDB6-4686-AF71-D9972AD5BB61}">
+L001=NA
+L002=Lubuk Naga
+L003=Jakarta
+L004=Ajibata
+L005=Pangambatan
+L006=Lontung
+L007=Sirungkungon
+L008=Silimalombu</text>
+  </threadedComment>
+  <threadedComment ref="H1" dT="2022-11-25T02:10:51.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{EC6CFADB-FDB6-4686-AF71-D9972AD5BB61}">
     <text>Value: Code Reference dengan reference type = Area
-ex: A001</text>
-  </threadedComment>
-  <threadedComment ref="H1" dT="2022-11-25T02:12:11.75" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{6E6F1860-48D6-4180-9BFB-66CD56B5D00D}">
+A001=NA
+A002=Processing Plant
+A003=Office	
+A004=Guest House
+A005=Feedmill	
+A006=Hatchery	
+A007=Landing Site 1	
+A008=Landing Site 2</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2022-11-25T02:12:11.75" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{6E6F1860-48D6-4180-9BFB-66CD56B5D00D}">
     <text>length: 500 character</text>
   </threadedComment>
-  <threadedComment ref="I1" dT="2022-11-25T02:12:58.72" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{F0908237-959A-4F39-92C9-6A75562F1BCE}">
+  <threadedComment ref="J1" dT="2022-12-08T02:35:07.54" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{F5D6FFB8-1100-4175-BD9B-B2031848A574}">
+    <text>Length: 50 character</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2022-11-25T02:12:58.72" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{F0908237-959A-4F39-92C9-6A75562F1BCE}">
     <text>Value: Code Reference dengan reference type = Asset Type
-ex: S001</text>
-  </threadedComment>
-  <threadedComment ref="J1" dT="2022-11-25T02:13:25.53" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{01DD0CBD-7AFB-4A0C-B267-9699F5EA165B}">
+S001=NA
+S002=Laptop
+S003=Printer Wirelless
+S004=Projector
+S005=Router
+S006=Access Point
+S007=UPS
+S008=Switch 10/100/1000
+S009=Camera Coaxial
+S010=Camera IP
+S011=DVR
+S012=NVR
+S013=Switch 10/100
+S014=Module SFP
+S015=Module Converter (MC)
+S016=Printer
+S017=Printer Lan
+S018=Stabillizer
+S019=HDD Casing 2.4
+S020=HDD Casing 3.5
+S021=Server</text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2022-11-25T02:13:25.53" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{01DD0CBD-7AFB-4A0C-B267-9699F5EA165B}">
     <text>Value: Code Reference dengan reference type = Asset Brand
-ex: B001</text>
-  </threadedComment>
-  <threadedComment ref="K1" dT="2022-11-25T02:14:03.96" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{74CC5E81-7BB4-4CB2-995E-9C13663A6644}">
+B001=NA
+B002=Lenovo
+B003=Asus
+B004=Acer
+B005=HP
+B006=Samsung
+B007=Orico
+B008=Bardi
+B009=IBM
+B010=Fortinet
+B011=Mikrotik
+B012=Unifi
+B013=TP-Link
+B014=D-Link
+B015=Ruijie
+B016=Huawei</text>
+  </threadedComment>
+  <threadedComment ref="M1" dT="2022-11-25T02:14:03.96" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{74CC5E81-7BB4-4CB2-995E-9C13663A6644}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="L1" dT="2022-11-25T02:14:10.86" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{C6E515DF-DF5A-4B4B-B861-A5F9089F4CB5}">
+  <threadedComment ref="N1" dT="2022-11-25T02:14:10.86" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{C6E515DF-DF5A-4B4B-B861-A5F9089F4CB5}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="M1" dT="2022-11-25T02:14:19.40" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{AAB51C24-7FFF-4657-8871-6FE7E675B9C6}">
+  <threadedComment ref="O1" dT="2022-11-25T02:14:19.40" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{AAB51C24-7FFF-4657-8871-6FE7E675B9C6}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="N1" dT="2022-11-25T02:16:38.31" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{B2684FF3-88DA-4455-8EDD-D82B4A8F8C5B}">
+  <threadedComment ref="P1" dT="2022-12-08T02:35:12.83" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{E0EE542A-2B38-4FD5-BE35-265C6F9707CE}">
+    <text>Length: 50 character</text>
+  </threadedComment>
+  <threadedComment ref="Q1" dT="2022-11-25T02:16:38.31" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{B2684FF3-88DA-4455-8EDD-D82B4A8F8C5B}">
     <text>Value: Code Reference dengan reference type = Color
-ex: C001</text>
-  </threadedComment>
-  <threadedComment ref="O1" dT="2022-11-25T02:17:43.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{45BDAA8A-9287-4EFC-B868-B765A2E24A0D}">
+C001=NA
+C002=Red
+C003=Black
+C004=White
+C005=Yellow
+C006=Green
+C007=Blue
+C008=Transparant
+C009=Silver
+C010=Grey
+C011=Brown</text>
+  </threadedComment>
+  <threadedComment ref="R1" dT="2022-11-25T02:17:43.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{45BDAA8A-9287-4EFC-B868-B765A2E24A0D}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="P1" dT="2022-11-25T02:17:48.46" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{DF51428B-CFC3-4522-8211-C03B9053A0C5}">
+  <threadedComment ref="S1" dT="2022-11-25T02:17:48.46" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{DF51428B-CFC3-4522-8211-C03B9053A0C5}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="Q1" dT="2022-11-25T02:17:23.26" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7EC55F5A-57D1-4574-BF47-D7C5393AEC8A}">
+  <threadedComment ref="T1" dT="2022-11-25T02:17:23.26" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7EC55F5A-57D1-4574-BF47-D7C5393AEC8A}">
     <text>Value: Code Reference dengan reference type = Touch Screen
-ex: U001</text>
-  </threadedComment>
-  <threadedComment ref="R1" dT="2022-11-25T02:18:07.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{B9A66794-AAE1-42F0-8013-9919087BCA06}">
+U001=NA
+U002=Yes
+U003=No</text>
+  </threadedComment>
+  <threadedComment ref="U1" dT="2022-11-25T02:18:07.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{B9A66794-AAE1-42F0-8013-9919087BCA06}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="S1" dT="2022-11-25T02:17:59.34" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{DDED7A91-AA30-4D58-AAA0-043D8C86F9FB}">
+  <threadedComment ref="V1" dT="2022-11-25T02:17:59.34" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{DDED7A91-AA30-4D58-AAA0-043D8C86F9FB}">
     <text>Value: Code Reference dengan reference type = VGA Brand
-ex: V001</text>
-  </threadedComment>
-  <threadedComment ref="T1" dT="2022-11-25T02:19:09.60" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{2095BA9B-35A9-4335-900C-D1B5D9E993DC}">
+V001=NA
+V002=NVidia
+V003=Radeon
+V004=ATI Radeon
+V005=Intel Iris
+V006=Intel</text>
+  </threadedComment>
+  <threadedComment ref="W1" dT="2022-11-25T02:19:09.60" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{2095BA9B-35A9-4335-900C-D1B5D9E993DC}">
     <text>Value: Code Reference dengan reference type = VGA Type
-ex: G001</text>
-  </threadedComment>
-  <threadedComment ref="U1" dT="2022-11-25T02:20:03.00" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{D517ECB9-A8D2-44AB-8307-4A81DD24DF09}">
+G001=NA
+G002=DDR4
+G003=DDR5</text>
+  </threadedComment>
+  <threadedComment ref="X1" dT="2022-11-25T02:20:03.00" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{D517ECB9-A8D2-44AB-8307-4A81DD24DF09}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="V1" dT="2022-11-25T02:24:50.03" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{1725C053-09E3-4137-838D-10A62C6E1FB7}">
+  <threadedComment ref="Y1" dT="2022-11-25T02:24:50.03" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{1725C053-09E3-4137-838D-10A62C6E1FB7}">
     <text>Value: Code Reference dengan reference type = RAM Type
-ex: R001</text>
-  </threadedComment>
-  <threadedComment ref="W1" dT="2022-11-25T02:23:27.83" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A4CF5CBF-0D29-4906-9E59-F15A66C189B6}">
+R001=NA
+R002=DDR
+R003=DDR2
+R004=DDR3
+R005=DDR3L
+R006=DDR4
+R007=DDR5</text>
+  </threadedComment>
+  <threadedComment ref="Z1" dT="2022-11-25T02:23:27.83" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A4CF5CBF-0D29-4906-9E59-F15A66C189B6}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="X1" dT="2022-11-25T02:23:39.99" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{38DDC78F-D356-4C96-A5A5-09E52D4E2997}">
+  <threadedComment ref="AA1" dT="2022-11-25T02:23:39.99" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{38DDC78F-D356-4C96-A5A5-09E52D4E2997}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="Y1" dT="2022-11-25T02:25:24.00" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{075415BC-24F5-4DF0-98AB-7B118D84DD9E}">
+  <threadedComment ref="AB1" dT="2022-11-25T02:25:24.00" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{075415BC-24F5-4DF0-98AB-7B118D84DD9E}">
     <text>Value: Code Reference dengan reference type = Storage Type
-ex: T001</text>
-  </threadedComment>
-  <threadedComment ref="Z1" dT="2022-11-25T02:26:02.91" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{2856AB68-D1EA-4362-B4C4-29E912499609}">
+T001=NA
+T002=HDD
+T003=SSD SATA
+T004=SSD NVME
+T005=SSD M.2</text>
+  </threadedComment>
+  <threadedComment ref="AC1" dT="2022-11-25T02:26:02.91" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{2856AB68-D1EA-4362-B4C4-29E912499609}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="AA1" dT="2022-11-25T02:27:24.75" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{F0769AF9-C4CA-4934-AA23-2EAD37E490F5}">
+  <threadedComment ref="AD1" dT="2022-11-25T02:27:24.75" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{F0769AF9-C4CA-4934-AA23-2EAD37E490F5}">
     <text>Value: Code Reference dengan reference type = Charger Type
-ex: H001</text>
-  </threadedComment>
-  <threadedComment ref="AB1" dT="2022-11-25T02:26:07.59" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{AF93CD7A-3953-4AA0-B8DE-11E97FF8EB47}">
+H001=NA
+H002=KW
+H003=ORIGINAL</text>
+  </threadedComment>
+  <threadedComment ref="AE1" dT="2022-11-25T02:26:07.59" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{AF93CD7A-3953-4AA0-B8DE-11E97FF8EB47}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="AC1" dT="2022-11-25T02:28:16.41" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7F72F8FD-20FF-47DF-8A5A-95CE7058FC86}">
+  <threadedComment ref="AF1" dT="2022-11-25T02:28:16.41" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7F72F8FD-20FF-47DF-8A5A-95CE7058FC86}">
     <text>Type Numeric(10,4) (Ex: 10.45)</text>
   </threadedComment>
-  <threadedComment ref="AD1" dT="2022-11-25T02:28:20.22" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{9FB7C414-E930-42FA-BF5F-1858645CA7FE}">
+  <threadedComment ref="AG1" dT="2022-11-25T02:28:20.22" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{9FB7C414-E930-42FA-BF5F-1858645CA7FE}">
     <text>Type Numeric(10,4) (Ex: 10.45)</text>
   </threadedComment>
-  <threadedComment ref="AE1" dT="2022-11-25T02:29:03.87" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{FF0B3A1E-E657-4B84-8260-6CAE71429588}">
+  <threadedComment ref="AH1" dT="2022-11-25T02:29:03.87" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{FF0B3A1E-E657-4B84-8260-6CAE71429588}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="AF1" dT="2022-11-25T02:26:16.95" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7ADE5977-2A89-45C2-8D2A-2A2B9E8BF5FB}">
+  <threadedComment ref="AI1" dT="2022-11-25T02:26:16.95" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7ADE5977-2A89-45C2-8D2A-2A2B9E8BF5FB}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="AG1" dT="2022-11-25T02:28:35.07" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{D2759B04-5250-467C-B703-A7DEB69F88A6}">
+  <threadedComment ref="AJ1" dT="2022-11-25T02:28:35.07" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{D2759B04-5250-467C-B703-A7DEB69F88A6}">
     <text>Type Numeric(10,4) (Ex: 10.45)</text>
   </threadedComment>
-  <threadedComment ref="AH1" dT="2022-11-25T02:26:29.53" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{C94C18E7-FE0D-4823-BD39-A2770272C0AF}">
+  <threadedComment ref="AK1" dT="2022-11-25T02:26:29.53" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{C94C18E7-FE0D-4823-BD39-A2770272C0AF}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="AI1" dT="2022-11-25T02:29:21.24" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{348202B7-A2B1-418B-868E-8D959F449C25}">
+  <threadedComment ref="AL1" dT="2022-11-25T02:29:21.24" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{348202B7-A2B1-418B-868E-8D959F449C25}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="AJ1" dT="2022-11-25T02:30:10.26" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A428C808-FB23-4D94-8784-ABA1CEE99BDD}">
+  <threadedComment ref="AM1" dT="2022-11-25T02:30:10.26" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A428C808-FB23-4D94-8784-ABA1CEE99BDD}">
     <text>Value: Code Reference dengan reference type = Chasing Type
-ex: N001</text>
-  </threadedComment>
-  <threadedComment ref="AK1" dT="2022-11-25T02:29:40.41" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{60EF7FD3-3C14-42CD-B72B-D2C5F8E0620D}">
+N001=NA
+N002=Micro
+N003=Mini
+N004=Medium
+N005=Full</text>
+  </threadedComment>
+  <threadedComment ref="AN1" dT="2022-11-25T02:29:40.41" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{60EF7FD3-3C14-42CD-B72B-D2C5F8E0620D}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="AL1" dT="2022-11-25T02:30:26.68" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{8C293A15-0351-42E6-8CA8-98C96A5A6B59}">
+  <threadedComment ref="AO1" dT="2022-11-25T02:30:26.68" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{8C293A15-0351-42E6-8CA8-98C96A5A6B59}">
     <text>Type Integer (Ex: 10)</text>
   </threadedComment>
-  <threadedComment ref="AM1" dT="2022-11-25T02:30:49.89" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{7A3E5C77-11E5-43C4-9BB3-57FF362712F0}">
-    <text>Value: Code Reference dengan reference type = Health
-ex: E001</text>
-  </threadedComment>
-  <threadedComment ref="AN1" dT="2022-11-25T02:31:34.48" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A09E11A4-C76F-4A0C-859C-FA187A5EB275}">
+  <threadedComment ref="AP1" dT="2022-11-25T02:31:34.48" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{A09E11A4-C76F-4A0C-859C-FA187A5EB275}">
     <text>Value: Code Reference dengan reference type = Operating System
-ex: O001</text>
-  </threadedComment>
-  <threadedComment ref="AO1" dT="2022-11-25T02:32:50.59" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{FFFADD91-B16E-4BB6-A356-9441A872E4DC}">
+O001=NA
+O002=Windows 7
+O003=Windows 8
+O004=Windows 8.1
+O005=Windows 10
+O006=Windows 11
+O007=Windows Ce
+O008=Windows Server 2008
+O009=Windows Server 2008 R2
+O010=Windows Server 2012
+O011=Windows Server 2012 R2
+O012=Windows Server 2016
+O013=Windows Server 2016 R2
+O014=Linux Centos
+O015=VMware Esxi 6.7.0
+O016=VMware Esxi 6.5.0</text>
+  </threadedComment>
+  <threadedComment ref="AQ1" dT="2022-11-25T02:32:50.59" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{FFFADD91-B16E-4BB6-A356-9441A872E4DC}">
     <text>Length: 300 character</text>
   </threadedComment>
-  <threadedComment ref="AP1" dT="2022-11-25T02:32:57.13" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{43733F07-F0C8-44AA-9B73-7EF3968FCF36}">
+  <threadedComment ref="AR1" dT="2022-11-25T02:32:57.13" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{43733F07-F0C8-44AA-9B73-7EF3968FCF36}">
     <text>Length: 30 character</text>
   </threadedComment>
-  <threadedComment ref="AQ1" dT="2022-11-25T02:33:03.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{17AC62A8-155A-4950-9CF9-9B05E6C208B0}">
+  <threadedComment ref="AS1" dT="2022-11-25T02:33:03.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{17AC62A8-155A-4950-9CF9-9B05E6C208B0}">
     <text>Length: 30 character</text>
   </threadedComment>
-  <threadedComment ref="AR1" dT="2022-11-25T02:33:14.63" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{00B93DB6-64C2-4327-ABF2-D95ED41C5701}">
+  <threadedComment ref="AT1" dT="2022-11-25T02:33:14.63" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{00B93DB6-64C2-4327-ABF2-D95ED41C5701}">
     <text>Length: 30 character</text>
   </threadedComment>
-  <threadedComment ref="AS1" dT="2022-11-25T02:33:23.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{95761249-7F6D-48C5-A51E-6F025B5E6978}">
+  <threadedComment ref="AU1" dT="2022-11-25T02:33:23.79" personId="{B454E715-2E34-4181-B687-C2802F0FA090}" id="{95761249-7F6D-48C5-A51E-6F025B5E6978}">
     <text>Length: 500 character</text>
   </threadedComment>
 </ThreadedComments>
@@ -1120,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD97E317-5A98-407F-9C59-B1011D36E470}">
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:AU1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK6" sqref="AK6"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1133,7 +1373,7 @@
     <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,126 +1387,132 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>